<commit_message>
Automatizado para la busqueda de todos los productos en ambos super, falta optimizar tiempo de busqueda, organizar mejor el excel
</commit_message>
<xml_diff>
--- a/excel/compras_mensuales_cod_supermas.xlsx
+++ b/excel/compras_mensuales_cod_supermas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IDEAPAD\Desktop\buscador\productFinder\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IDEAPAD\Desktop\buscador\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FDF840-4F2F-49EA-A144-F22198664AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F58B342-883C-4AED-8EE4-A7AEAE58E6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Productos</t>
   </si>
@@ -44,24 +44,6 @@
     <t>Santa</t>
   </si>
   <si>
-    <t>Fideo Federeal Tallarin Grueso</t>
-  </si>
-  <si>
-    <t>Azucar Morena Eco Agro 2Kg</t>
-  </si>
-  <si>
-    <t>Papel Higienico Bio premiun de 30m x 12 rollos</t>
-  </si>
-  <si>
-    <t>Bolsa de Basura de 200 lts resistente</t>
-  </si>
-  <si>
-    <t>Bolsa de Basura de 100 lts resistente</t>
-  </si>
-  <si>
-    <t>Bolsa de basura chico p/baño</t>
-  </si>
-  <si>
     <t>Ladis</t>
   </si>
   <si>
@@ -74,54 +56,9 @@
     <t>Cesar</t>
   </si>
   <si>
-    <t>Lavandina Power Abba de 5 lts</t>
-  </si>
-  <si>
-    <t>Detergente power Abba de 5 lts</t>
-  </si>
-  <si>
-    <t>Desodorante de Ambiente Power Abba 5 lts</t>
-  </si>
-  <si>
-    <t>Desodarante Nivea roll on men</t>
-  </si>
-  <si>
-    <t>Fideo Federal Spaguetti de 400 gr</t>
-  </si>
-  <si>
-    <t>Jabon en polvo Cavallaro de 3 kg</t>
-  </si>
-  <si>
-    <t>Comida para Gato Cat Chow Adulto 1 kg</t>
-  </si>
-  <si>
-    <t>Harina Leudante Blanca Flor de 1 kg</t>
-  </si>
-  <si>
-    <t>Harina tipo 000 Mickey o Primicia 1 kg</t>
-  </si>
-  <si>
-    <t>Harina Salvado Mickey o Primicia 1 kg</t>
-  </si>
-  <si>
-    <t>Bolsa de Basura de 150 lts resistente</t>
-  </si>
-  <si>
-    <t>Desodarante Dove Aerosol</t>
-  </si>
-  <si>
-    <t>Desodarante Dove roll on</t>
-  </si>
-  <si>
     <t>Sergio</t>
   </si>
   <si>
-    <t>Comida para Gasto sabor Carne Whiskas 1 kg</t>
-  </si>
-  <si>
-    <t>Suavizante para ropa Power Abba de 5 lts</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -206,15 +143,6 @@
     <t>si es 6 unidades a Gs 6.413</t>
   </si>
   <si>
-    <t>LECHE LACTOLANDA LARGA VIDA DESCREMADA 1 LT</t>
-  </si>
-  <si>
-    <t>LECHE TREBOL ULTRA DESCREMADA SACHET 1 LT</t>
-  </si>
-  <si>
-    <t>LECHE LOS COLONOS TETRA DESCREMADA 1 LT</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 6.080</t>
   </si>
   <si>
@@ -224,15 +152,6 @@
     <t>si es 6 unidades a Gs 7.553</t>
   </si>
   <si>
-    <t>LECHE TREBOL LARGA VIDA ENTERA 1 LT</t>
-  </si>
-  <si>
-    <t>LECHE LACTOLANDA LARGA VIDA ENTERA 1 LT</t>
-  </si>
-  <si>
-    <t>LECHE LOS COLONOS TETRA ENTERA 1 LT</t>
-  </si>
-  <si>
     <t>LECHE TREBOL SIN LACTOSA UAT 1 LT</t>
   </si>
   <si>
@@ -272,46 +191,25 @@
     <t>SAL MARINA ENTREFINA MICKEY 500 GR</t>
   </si>
   <si>
-    <t>SAL MARINA ARCOIRIS GRUESA 500GR</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 3.610</t>
   </si>
   <si>
     <t>si es 6 unidades a Gs 4.180</t>
   </si>
   <si>
-    <t>SHAMPOO CLEAR 2 EN 1 DUAL EFFECT 400 ML</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 33.725</t>
   </si>
   <si>
-    <t>SHAMPOO SEDAL CASPA CONTROL 340ML</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 18.383</t>
   </si>
   <si>
-    <t>POMPITA FRAGANCIAS DE AZAHAR 1,5LT</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 15.295</t>
   </si>
   <si>
-    <t>YERBA M CAMPESINO MENTA Y BOLDO 500GR</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 9.738</t>
   </si>
   <si>
-    <t>YERBA CAMPESINO REFRESC 500GR</t>
-  </si>
-  <si>
     <t>si es 6 unidades a Gs 10.260</t>
-  </si>
-  <si>
-    <t>YERBA INDEGA PLASTICO 1 KG</t>
   </si>
   <si>
     <t>si es 6 unidades a Gs 14.915</t>
@@ -717,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +628,7 @@
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -739,25 +637,25 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -765,7 +663,7 @@
         <v>7790272001029</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -792,7 +690,7 @@
         <v>7840997000019</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -816,7 +714,7 @@
         <v>7792170000708</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -835,12 +733,15 @@
         <v>18150</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>7891000016602</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -856,9 +757,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>7</v>
+    <row r="8" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>7840112001228</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -868,9 +772,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>6</v>
+    <row r="9" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>7840127000759</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -880,9 +787,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>22</v>
+    <row r="10" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>7840024005413</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -892,9 +802,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>5</v>
+    <row r="11" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>7840024005253</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -912,10 +825,10 @@
     </row>
     <row r="12" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>7891000016602</v>
+        <v>7790040669208</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -932,11 +845,11 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <v>7840112001228</v>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -949,11 +862,14 @@
         <v>10200</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>7790990587867</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D14">
@@ -964,9 +880,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>18</v>
+    <row r="15" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>2000510000000</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -976,9 +895,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>23</v>
+    <row r="16" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>7840003023087</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -991,9 +913,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>24</v>
+    <row r="17" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>7509546657110</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1003,9 +928,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>15</v>
+    <row r="18" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>7794000006164</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -1015,9 +943,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>14</v>
+    <row r="19" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>7840005012416</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1033,9 +964,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>13</v>
+    <row r="20" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>7840005012690</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1053,10 +987,10 @@
     </row>
     <row r="21" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>7840127000759</v>
+        <v>7840037000917</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1075,15 +1009,15 @@
         <v>15550</v>
       </c>
       <c r="M21" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
-        <v>7840024005413</v>
+        <v>7840833000630</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1096,15 +1030,15 @@
         <v>4650</v>
       </c>
       <c r="M22" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>7840024005253</v>
+        <v>7794000006430</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1120,12 +1054,15 @@
         <v>4650</v>
       </c>
       <c r="M23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>7791866001579</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -1138,9 +1075,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>2</v>
+    <row r="25" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>7841390000156</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1155,10 +1095,10 @@
     </row>
     <row r="26" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
-        <v>7790040669208</v>
+        <v>7891024005064</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1177,12 +1117,15 @@
         <v>11200</v>
       </c>
       <c r="M26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>7840029875059</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1192,9 +1135,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>21</v>
+    <row r="28" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>7840100314286</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1205,9 +1151,6 @@
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
       <c r="F29">
         <v>1</v>
       </c>
@@ -1216,13 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>45</v>
-      </c>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="G30">
         <v>2</v>
       </c>
@@ -1237,16 +1174,10 @@
         <v>27850</v>
       </c>
       <c r="M30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B31" s="1">
-        <v>7790990587867</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F31">
         <v>6</v>
       </c>
@@ -1264,13 +1195,10 @@
         <v>12300</v>
       </c>
       <c r="M31" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
       <c r="G32">
         <v>2</v>
       </c>
@@ -1279,13 +1207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B33" s="1">
-        <v>2000510000000</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>49</v>
-      </c>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F33">
         <v>1</v>
       </c>
@@ -1300,13 +1222,7 @@
         <v>12750</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B34" s="1">
-        <v>7840003023087</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>50</v>
-      </c>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D34">
         <v>3</v>
       </c>
@@ -1318,16 +1234,10 @@
         <v>11850</v>
       </c>
       <c r="M34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B35" s="1">
-        <v>7509546657110</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F35">
         <v>1</v>
       </c>
@@ -1345,16 +1255,10 @@
         <v>26400</v>
       </c>
       <c r="M35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B36" s="1">
-        <v>7794000006164</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F36">
         <v>3</v>
       </c>
@@ -1372,13 +1276,10 @@
         <v>15350</v>
       </c>
       <c r="M36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F37">
         <v>1</v>
       </c>
@@ -1393,13 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B38" s="1">
-        <v>7840042000124</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>56</v>
-      </c>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F38">
         <v>4</v>
       </c>
@@ -1414,44 +1309,26 @@
         <v>6700</v>
       </c>
       <c r="M38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B39" s="1">
-        <v>7840005012409</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>57</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
       <c r="L39">
         <v>6750</v>
       </c>
       <c r="M39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B40" s="1">
-        <v>7840037001310</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
       <c r="L40">
         <v>6400</v>
       </c>
       <c r="M40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B41" s="1">
-        <v>7840005012379</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
       <c r="G41">
         <v>5</v>
       </c>
@@ -1463,44 +1340,26 @@
         <v>6750</v>
       </c>
       <c r="M41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B42" s="1">
-        <v>7840042000117</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
       <c r="L42">
         <v>6700</v>
       </c>
       <c r="M42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B43" s="1">
-        <v>7840037001204</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
       <c r="L43">
         <v>6400</v>
       </c>
       <c r="M43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B44" s="1">
-        <v>7840005012416</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.3">
       <c r="G44">
         <v>4</v>
       </c>
@@ -1512,16 +1371,10 @@
         <v>7950</v>
       </c>
       <c r="M44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B45" s="1">
-        <v>7840005012690</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F45">
         <v>4</v>
       </c>
@@ -1533,30 +1386,18 @@
         <v>7500</v>
       </c>
       <c r="M45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B46" s="1">
-        <v>7840037000917</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.3">
       <c r="L46">
         <v>7400</v>
       </c>
       <c r="M46" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B47" s="1">
-        <v>7840833000630</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F47">
         <v>1</v>
       </c>
@@ -1568,16 +1409,10 @@
         <v>6200</v>
       </c>
       <c r="M47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B48" s="1">
-        <v>7794000006430</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>95</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
       <c r="G48">
         <v>1</v>
       </c>
@@ -1592,16 +1427,10 @@
         <v>16750</v>
       </c>
       <c r="M48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B49" s="1">
-        <v>7791866001579</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F49">
         <v>3</v>
       </c>
@@ -1610,13 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B50" s="1">
-        <v>7841390000156</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>72</v>
-      </c>
+    <row r="50" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F50">
         <v>1</v>
       </c>
@@ -1634,13 +1457,10 @@
         <v>6550</v>
       </c>
       <c r="M50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D51">
         <v>1</v>
       </c>
@@ -1658,13 +1478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B52" s="1">
-        <v>7891024005064</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>73</v>
-      </c>
+    <row r="52" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F52">
         <v>2</v>
       </c>
@@ -1682,16 +1496,10 @@
         <v>30300</v>
       </c>
       <c r="M52" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B53" s="1">
-        <v>7840029875059</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F53">
         <v>5</v>
       </c>
@@ -1703,16 +1511,10 @@
         <v>4950</v>
       </c>
       <c r="M53" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B54" s="1">
-        <v>7840100314286</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>77</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D54">
         <v>1</v>
       </c>
@@ -1733,16 +1535,10 @@
         <v>3800</v>
       </c>
       <c r="M54" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B55" s="1">
-        <v>7840595013114</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>78</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D55">
         <v>1</v>
       </c>
@@ -1757,16 +1553,10 @@
         <v>4400</v>
       </c>
       <c r="M55" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B56" s="1">
-        <v>7501056342999</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>81</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="4:13" x14ac:dyDescent="0.3">
       <c r="G56">
         <v>2</v>
       </c>
@@ -1778,16 +1568,10 @@
         <v>35500</v>
       </c>
       <c r="M56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B57" s="1">
-        <v>7791293045788</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F57">
         <v>2</v>
       </c>
@@ -1799,16 +1583,10 @@
         <v>19350</v>
       </c>
       <c r="M57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B58" s="1">
-        <v>7840033008474</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="4:13" x14ac:dyDescent="0.3">
       <c r="G58">
         <v>2</v>
       </c>
@@ -1820,13 +1598,10 @@
         <v>16100</v>
       </c>
       <c r="M58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>27</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F59">
         <v>1</v>
       </c>
@@ -1835,13 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B60" s="1">
-        <v>7840009650072</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>87</v>
-      </c>
+    <row r="60" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F60">
         <v>1</v>
       </c>
@@ -1853,16 +1622,10 @@
         <v>10250</v>
       </c>
       <c r="M60" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B61" s="1">
-        <v>7840009650058</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>89</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.3">
       <c r="F61">
         <v>2</v>
       </c>
@@ -1874,16 +1637,10 @@
         <v>10800</v>
       </c>
       <c r="M61" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B62" s="1">
-        <v>7840045018546</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.3">
       <c r="G62">
         <v>1</v>
       </c>
@@ -1898,7 +1655,7 @@
         <v>15700</v>
       </c>
       <c r="M62" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>